<commit_message>
ver 2: lastest update
</commit_message>
<xml_diff>
--- a/DesktopApp/bin/Debug/file/ExportExcelCSR.Dialog.xlsx
+++ b/DesktopApp/bin/Debug/file/ExportExcelCSR.Dialog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOBILE ID\HoTroKH_TichHopRSSP\DesktopApplicationTool\DesktopApp\DesktopApp\bin\Debug\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gia\Documents\Visual Studio 2022\DesktopApplicationToolVer_1\DesktopApp\bin\Debug\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED52BAB3-822C-4A35-AE05-1DA016671E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ToolResult" sheetId="1" r:id="rId1"/>
@@ -33,41 +34,115 @@
     <t>Cert Chain</t>
   </si>
   <si>
-    <t xml:space="preserve">"-----BEGIN CERTIFICATE REQUEST-----
+    <t xml:space="preserve">-----BEGIN CERTIFICATE REQUEST-----
 MIICtDCCAZwCAQAwcTEVMBMGA1UEAwwMTmd1eWVuIFZhbiBCMRQwEgYDVQQLDAtD
 b25nIFR5IEFCQzEUMBIGA1UECgwLQ29uZyBUeSBBQkMxCzAJBgNVBAYTAlZOMQ8w
 DQYDVQQHDAZRdWFuIDExDjAMBgNVBAgMBVRQSENNMIIBIjANBgkqhkiG9w0BAQEF
-AAOCAQ8AMIIBCgKCAQEAhmrWdY6lMzD13kUxayQsAO09woiNxfkTn+Z28hqm8CvR
-yUZcsNjXUAvCgCKOqjdmMQLFyer7BTDmQtyZE5Y8X3aVtnkvLOCEehYfsRaSekKe
-Ohc4K3S/DtGEIfNNm5iPpbuKhJ7W91R5Dr2i07fEThYyGgB/UvypkGqjP0qQDWj+
-3Vt06/tJqe8JQE7f/K6MfX2YGXLbWJ4iX0473y7iuLq5wGGfE4dlYVcCiJYWLTti
-II29NwUbs8u6QSLZ/O0TFaQwb1r6sRTtO9hOgZ0f8qER0LvXQWjWXTbbFVSEn9iJ
-5pWtT8ABzZC2P92+0qfbcsyW7fQ0UWvXvZvFHwkpIQIDAQABMA0GCSqGSIb3DQEB
-BQUAA4IBAQB19J+jtnbNv+FYWHpLIs3iFoHIX49tgVTDgeTN5VpSZYuTuc+Sdo7N
-Z3K0G0G+AW7gzEkF6YqrPzE7dk8C6W22+yHMFARVMB5QEgDot1XGfn7iRsVTLIjn
-iJxlpB9IE9UIaGB6ONKIvupaEncJbUxRWBISMuY/sDv3Sxv1vgcoHsCEAVvVKyfr
-VPzLBJ4Fz63qHMiAphf9+WAbWE/MQwFBHcdoyXM1067XBSD3vMHyXHmeXMPx43c1
-7Fm3gddsd6sFhcnDRvHxYosiTU0glCOze/o8vgOrONJHDkQ3amnPYjpapgTku1Gm
-IIFdxxbcLC8IEfShvQSEOiIeOpR3iIUp
------END CERTIFICATE REQUEST-----"
+AAOCAQ8AMIIBCgKCAQEApqrDZWbKR/SZQgn9PDPvuQgFks5xvAeCB1lOYMS2748V
+hkviZrGwwpmgsuot1QRwPgaRoP4P9jSIBWEpwOtM7SBYIhDWQHqzwb3Z7aarpITE
+DWb+zDlDeTDRT5ITLxwmcOOz4sxIcHQ8EMTQP5NjZVxwQaTsSApjoMahhQIgUvoh
++1NQb1XTLXSu2nmpzji/T48e5Wrmrhp8Y+Cs/LEcHLdLV9zsGna0KjrQxjaqXYTq
+e5OaWg3xoBNpyCKvwelJC02aft6A0DVEBRzJC0XKwGM4jYAwD+HWRWd+8JVyQqZQ
+6uYO4Rc94H2thf8kq7/1f2MSgKkGY4uEv5QmNmH8NwIDAQABMA0GCSqGSIb3DQEB
+BQUAA4IBAQCKL9JbHICtl0XlrKkUNCwg9MAnaCj5UR6PfnWsNG43dfJ9CCQ7wpWj
+auA61RF+3l9LXNK5669QeigCs0ewOBXtEo27uhaLtNE17fpUG7dAI46PJV7/AqXm
+4SMXLoU1gjZdtUU40GjxTq6Qxa1bchVKCOXHE4XAYmA5WOxtV4YmJCGTZvqOhrOl
+5MJixG27f0lNFT0nd/ELj2jwrQD1cNarX6THNOG/i12B6Dpad3qh3NpOjjsiADvc
+x/ewr0H9VctqHd1SQNi0d2bEtaHBr7jw/DANtwgcdccqzkIymScvqAtX8oRac1du
+y7xr4nN0Q85pvKwdXY9AxHSF7Vrd43pq
+-----END CERTIFICATE REQUEST-----
 </t>
   </si>
   <si>
-    <t>MIIGRDCCBCygAwIBAgIEVfAPITANBgkqhkiG9w0BAQsFADCByDELMAkGA1UEBhMCVk4xFDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFAMD4GA1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9pbnQgU3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBEZXBhcnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMCAXDTE3MDQyMTAyNTA1MVoYDzIxMTcwMzI4MDI1MDUxWjCByDELMAkGA1UEBhMCVk4xFDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFAMD4GA1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9pbnQgU3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBEZXBhcnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMIICIjANBgkqhkiG9w0BAQEFAAOCAg8AMIICCgKCAgEAjtHJbKRUfVPE3vr7SjROLgQYO1bTi+WgIinSsLn9XGj7gjO4cx8ejs9I8IGrx2q5Wzcrcavi5nxRzoKbO8EVkR+F69UxgF54e8Nfe76i3v8BGTk8vngpvQrndN8uE6YiQ/G0s5hLi/gZfffcMTlMQrlwYdRpEMhn6nNoF675xpaBk15+epa7SjXbgGvCkA0CkR+SKvhd4pnMORZ2/jpQvLG5DQIzQLApAmWHcoexFxTgPzuw2qhinWPO07X/H5pz5dAAKhflI451OG2PZCloZEo1lemmspm3azFlaYzkbLPI+GsV61PB/AQEIKq9tXLCuyYbpXYqOlbFP8LYGyfumdOwS2/LFKwHGLAdlofCGI0eMp/dsa+aL+My8Rqv0S0PhClcnvDaSCIYBPDgI5wW4u/sr3Wz5n5f4Z3k5vJi0GU8l0FroNsFCN8EOc/vM+wgm+Uol74FrEo0LpT8TUWh71HUF29sBxtEQ8Zw5YpUMCTcPuBsVRwuLGGae8VKpPc4jEwpGmvoGj8cfS2qoEMNPtRnGM3Kt+q39zLoDk+6Kmr5oi8XVfZmibXRtNvrixMj6jAEm/3Vag9VdQ4SR+QFwpJOcIOBtX9mDnamXnBHWFqGUqOUU9/6y4p8B2o3RDE/WeiWtU66gQZasli6TJb0RpNoY/XyXHGn+J0gd9EDXn0CAwEAAaMyMDAwDwYDVR0TAQH/BAUwAwEB/zAdBgNVHQ4EFgQU82QyfbI8XeUu4El8tOpiFZR4LqswDQYJKoZIhvcNAQELBQADggIBAI3hBTzed1ZtDh5DvdidSJoGRBXJQ24Y3VjxPbelLNxnZiYCiSIQhL7KIjmDZOBQJwqlBxWOsao7PuRaohdAcDQ2jImeiIAmkRaTcUWZgB++IuS1ta01XMcAEp/taQEjHKjwAr22IILNVk9z0WNVf5Pd9NWMu4lFqwECpKTJnToIqEGVVWcqAAupGT64LQ/Cf+/oEpDtkRaVazFj7ob1Rxjl5hmOxMwNHW8wRPcq8glg+26Tp9jqcaw32fhfnUPDHBdoYcU/VhMkgBeYXGHTPHp32Kj4l/QxWnxY0IvChyq+Qao1D19K5PbJQH5A5bQbwqgBtMihsdrGSr9VJ7LtNmBc+8dNchqi2uXs3ryk8htDluZ60yWK89eRO1NatB2tiDLh5iwejJRieOoyQ3Iq8m/IjtEJTs7ehWJHtiGj2U/tlpVW2fSszoz0TbKxXQPQ/dGNmDorqrM/0WEY6lkNEp7qbXB1U378PFUKFh1lIdlfNrgoEvYt0XeIMbXn+fUkB8munP0bCSiJqX7gK+2FuZqfA038JfuwxDBr8SvkkvZOqyUgMPAPRpQCjmFrZgMrilHUokZIL5+Cz4qaxEf3s3xORy+CuPMousfrOKpdf6jFjnyD8cr4Ez4bMAekPg4F4JJ0WHpOchSlDP5a57cb6mHYvOF8ygSobADyNeQ1jkjg</t>
-  </si>
-  <si>
-    <t>MIIGejCCBGKgAwIBAgIMTWIp3U9d251FXlVaMA0GCSqGSIb3DQEBCwUAMIHIMQswCQYDVQQGEwJWTjEUMBIGA1UECBMLSG8gQ2hpIE1pbmgxFDASBgNVBAcTC0hvIENoaSBNaW5oMUAwPgYDVQQKEzdNb2JpbGUtSUQgVGVjaG5vbG9naWVzIGFuZCBTZXJ2aWNlcyBKb2ludCBTdG9jayBDb21wYW55MScwJQYDVQQLEx5Nb2JpbGUtSUQgVGVjaG5pY2FsIERlcGFydG1lbnQxIjAgBgNVBAMTGU1vYmlsZS1JRCBUcnVzdGVkIE5ldHdvcmswHhcNMjIwODA0MDg1NDAwWhcNMjMwODA5MDg1NDAwWjCBpzELMAkGA1UEBhMCVk4xFzAVBgNVBAgMDkjhu5MgQ2jDrSBNaW5oMRgwFgYDVQQKDA9OZ3V5ZW4gVmFuIFRlc3QxFTATBgNVBAsMDENvbmcgVHkgQUJDRDEYMBYGA1UEAwwPTmd1eWVuIFZhbiBUZXN0MR8wHQYKCZImiZPyLGQBAQwPTVNUOjEyMzQ1Njc4MDA0MRMwEQYDVQQUEwowMTIzNDU2Nzg5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAhmrWdY6lMzD13kUxayQsAO09woiNxfkTn+Z28hqm8CvRyUZcsNjXUAvCgCKOqjdmMQLFyer7BTDmQtyZE5Y8X3aVtnkvLOCEehYfsRaSekKeOhc4K3S/DtGEIfNNm5iPpbuKhJ7W91R5Dr2i07fEThYyGgB/UvypkGqjP0qQDWj+3Vt06/tJqe8JQE7f/K6MfX2YGXLbWJ4iX0473y7iuLq5wGGfE4dlYVcCiJYWLTtiII29NwUbs8u6QSLZ/O0TFaQwb1r6sRTtO9hOgZ0f8qER0LvXQWjWXTbbFVSEn9iJ5pWtT8ABzZC2P92+0qfbcsyW7fQ0UWvXvZvFHwkpIQIDAQABo4IBgTCCAX0wDAYDVR0TAQH/BAIwADAfBgNVHSMEGDAWgBTzZDJ9sjxd5S7gSXy06mIVlHguqzByBggrBgEFBQcBAQRmMGQwMgYIKwYBBQUHMAKGJmh0dHBzOi8vbW9iaWxlLWlkLnZuL3BraS9tb2JpbGUtaWQuY3J0MC4GCCsGAQUFBzABhiJodHRwOi8vbW9iaWxlLWlkLnZuL29jc3AvcmVzcG9uZGVyMEUGA1UdIAQ+MDwwOgYLKwYBBAGB7QMBBAEwKzApBggrBgEFBQcCARYdaHR0cHM6Ly9tb2JpbGUtaWQudm4vY3BzLmh0bWwwNAYDVR0lBC0wKwYIKwYBBQUHAwIGCCsGAQUFBwMEBgorBgEEAYI3CgMMBgkqhkiG9y8BAQUwLAYDVR0fBCUwIzAhoB+gHYYbaHR0cDovL21vYmlsZS1pZC52bi9jcmwvZ2V0MB0GA1UdDgQWBBT2uDq+0cZWbcPlZHAB7ji3zr71ojAOBgNVHQ8BAf8EBAMCBPAwDQYJKoZIhvcNAQELBQADggIBACljlyNXjSYN1KCkD8k7t6Z0zm1LJfARu7YZfky0qtUwqaObLz3stl1LTPqb4ezF9p2e2JgJXqPqv9vs3J58iE30qzNma7OFd3es0JSn2ioUDqbbIw3tl8F1RW9a74cHnLtiBm8gRHNuJRk3zbwja9zBS4fCIsOX/4OGgpVHafqKCBSJ4AlxxY/oHYObcDZEfaR6ltwqAM1YF9ngj/0w87Lr/vtlT9Vte26ujE4FMSIDq9ct9vM9hIG6HYcLXRc7SqHXm6bnqGaDYTJzSnoexIkCwC5fwL35Q1UGIq8FG7WtepHznaXCDldatT0tRiwF2rpmP6yMWW3Z8H98BQOJx4J/khFWK2DVJxHKnlmvyhHDQvdIptwyPIaCDnNwWH2v6HeA2T7CRVbDo2s1la62aBi/96irHYX+GEgmuMP14cCP60Z6TMdfQ63QVcMKOF8Z27PzT//yYHWECnJLP+S3sKoaWbelPROSG1ecGrFYyt2CkHeQvfyduihNknpa8wwojXc82/mP2NcTbiuK1Sb4qAnn/h0m8XxkHMGoK1lxRcBQNrTJRkFCVJMTSBAo8QgnP9Z7FNSvimq7X3ahp5d4H6JTwji/k6bUw0k57yW27pKiuBu9bQxV6jkXZJmGPcRrRX8t2dubs+3cxLe8V81+a/2AILtb95J1yjtaijCiMhEq</t>
+    <t>"-----BEGIN CERTIFICATE-----
+MIIG6TCCBNGgAwIBAgIMO4PMpx9HUH7JUavKMA0GCSqGSIb3DQEBCwUAMIHIMQsw
+CQYDVQQGEwJWTjEUMBIGA1UECBMLSG8gQ2hpIE1pbmgxFDASBgNVBAcTC0hvIENo
+aSBNaW5oMUAwPgYDVQQKEzdNb2JpbGUtSUQgVGVjaG5vbG9naWVzIGFuZCBTZXJ2
+aWNlcyBKb2ludCBTdG9jayBDb21wYW55MScwJQYDVQQLEx5Nb2JpbGUtSUQgVGVj
+aG5pY2FsIERlcGFydG1lbnQxIjAgBgNVBAMTGU1vYmlsZS1JRCBUcnVzdGVkIE5l
+dHdvcmswHhcNMjIwODI2MDY1MDMxWhcNMjMwODI2MDY1MDMxWjCB9zELMAkGA1UE
+BhMCVk4xFDASBgNVBAgMC0Lhuq9jIEvhuqFuMRswGQYDVQQHDBI5MC80MyBMeU5h
+bURlUDdRMTExEjAQBgNVBAoMCU1vYmlsZS1JZDEMMAoGA1UEDAwDRGV2MRkwFwYD
+VQQDDBBU4bqldCBLaMOhbmggR2lhMR0wGwYKCZImiZPyLGQBAQwNTVNUOjAxMjM0
+NTY3MTEhMB8GCgmSJomT8ixkAQEMEUNNTkQ6MDc5MjAwMDExMTg5MSEwHwYJKoZI
+hvcNAQkBFhJnaWF0a0Btb2JpbGUtaWQudm4xEzARBgNVBBQTCjA1NjY0Nzc4NDcw
+ggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCmqsNlZspH9JlCCf08M++5
+CAWSznG8B4IHWU5gxLbvjxWGS+JmsbDCmaCy6i3VBHA+BpGg/g/2NIgFYSnA60zt
+IFgiENZAerPBvdntpqukhMQNZv7MOUN5MNFPkhMvHCZw47PizEhwdDwQxNA/k2Nl
+XHBBpOxICmOgxqGFAiBS+iH7U1BvVdMtdK7aeanOOL9Pjx7lauauGnxj4Kz8sRwc
+t0tX3OwadrQqOtDGNqpdhOp7k5paDfGgE2nIIq/B6UkLTZp+3oDQNUQFHMkLRcrA
+YziNgDAP4dZFZ37wlXJCplDq5g7hFz3gfa2F/ySrv/V/YxKAqQZji4S/lCY2Yfw3
+AgMBAAGjggGgMIIBnDAMBgNVHRMBAf8EAjAAMB8GA1UdIwQYMBaAFPNkMn2yPF3l
+LuBJfLTqYhWUeC6rMHIGCCsGAQUFBwEBBGYwZDAyBggrBgEFBQcwAoYmaHR0cHM6
+Ly9tb2JpbGUtaWQudm4vcGtpL21vYmlsZS1pZC5jcnQwLgYIKwYBBQUHMAGGImh0
+dHA6Ly9tb2JpbGUtaWQudm4vb2NzcC9yZXNwb25kZXIwHQYDVR0RBBYwFIESZ2lh
+dGtAbW9iaWxlLWlkLnZuMEUGA1UdIAQ+MDwwOgYLKwYBBAGB7QMBBAEwKzApBggr
+BgEFBQcCARYdaHR0cHM6Ly9tb2JpbGUtaWQudm4vY3BzLmh0bWwwNAYDVR0lBC0w
+KwYIKwYBBQUHAwIGCCsGAQUFBwMEBgorBgEEAYI3CgMMBgkqhkiG9y8BAQUwLAYD
+VR0fBCUwIzAhoB+gHYYbaHR0cDovL21vYmlsZS1pZC52bi9jcmwvZ2V0MB0GA1Ud
+DgQWBBRdlDDMORtdYxORKTRz/G14zuf3WzAOBgNVHQ8BAf8EBAMCBPAwDQYJKoZI
+hvcNAQELBQADggIBAF8aaYe4a/ZE5A4a7uTKkfkWWDrs/POMjQ/8sCazFiVkh9Ke
+hB/PZlT35l48oL7P9KrqiJLmBHZOwLemWCx4RkPqD7ylAg7Rm5/XFM56OuRPFhE3
+aaAbkbGuc4rqDxCUKw4XeLBp3wKwmS0jk8bDZzuxhocWIWc886aNQqxiudmr2XJK
+Im6RXbnLG24nGrOGhVvYV+ZDrZA5+I0Gsn0I12ZPMDo4SNefDKQE/y6KAbJKxpN6
+zdZMTymtp9H0KhjF8u07iXxEtkGqxhrffmDctNLwvPLP2wX1E92Z9TlzSevomTIV
+Rh5m3kZx3A6ZM+WVmiBGHhNPosh95LilWV0MX8L40oNFbJK9jAwoIgKhh32wvrHU
+cM23ZVWC0wACozUynv2Bl1gamYjS75CPtYvUvJPzw4W2ef2GCK+FybLo35pClr1o
+IbDw/yMtN+5oG6vgXDRbaOa28V5/zLglpe9WUr7I669yHTDK+IorShoAlE7/qT7d
+czwNIjz5Ft0x+kDubyM5dmH5K67CQfgql6u2ygTxSL+5/fHQ+lWNNkTdNEwV8Nf4
+GMWFbn62PVl+QKPPORWZRUh629NrxDNdwA6qriwus7tGk2QOjOzLlMNCSSozwgpz
+u+xBnWVKL+MH6ogV0BgW21geiKDV7rLR9z4D0SMSA/wUanufWUJckSGawaxC
+-----END CERTIFICATE-----"</t>
+  </si>
+  <si>
+    <t>"                                -----BEGIN CERTIFICATE-----
+MIIGRDCCBCygAwIBAgIEVfAPITANBgkqhkiG9w0BAQsFADCByDELMAkGA1UEBhMC
+Vk4xFDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFA
+MD4GA1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9p
+bnQgU3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBE
+ZXBhcnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMCAX
+DTE3MDQyMTAyNTA1MVoYDzIxMTcwMzI4MDI1MDUxWjCByDELMAkGA1UEBhMCVk4x
+FDASBgNVBAgTC0hvIENoaSBNaW5oMRQwEgYDVQQHEwtIbyBDaGkgTWluaDFAMD4G
+A1UEChM3TW9iaWxlLUlEIFRlY2hub2xvZ2llcyBhbmQgU2VydmljZXMgSm9pbnQg
+U3RvY2sgQ29tcGFueTEnMCUGA1UECxMeTW9iaWxlLUlEIFRlY2huaWNhbCBEZXBh
+cnRtZW50MSIwIAYDVQQDExlNb2JpbGUtSUQgVHJ1c3RlZCBOZXR3b3JrMIICIjAN
+BgkqhkiG9w0BAQEFAAOCAg8AMIICCgKCAgEAjtHJbKRUfVPE3vr7SjROLgQYO1bT
+i+WgIinSsLn9XGj7gjO4cx8ejs9I8IGrx2q5Wzcrcavi5nxRzoKbO8EVkR+F69Ux
+gF54e8Nfe76i3v8BGTk8vngpvQrndN8uE6YiQ/G0s5hLi/gZfffcMTlMQrlwYdRp
+EMhn6nNoF675xpaBk15+epa7SjXbgGvCkA0CkR+SKvhd4pnMORZ2/jpQvLG5DQIz
+QLApAmWHcoexFxTgPzuw2qhinWPO07X/H5pz5dAAKhflI451OG2PZCloZEo1lemm
+spm3azFlaYzkbLPI+GsV61PB/AQEIKq9tXLCuyYbpXYqOlbFP8LYGyfumdOwS2/L
+FKwHGLAdlofCGI0eMp/dsa+aL+My8Rqv0S0PhClcnvDaSCIYBPDgI5wW4u/sr3Wz
+5n5f4Z3k5vJi0GU8l0FroNsFCN8EOc/vM+wgm+Uol74FrEo0LpT8TUWh71HUF29s
+BxtEQ8Zw5YpUMCTcPuBsVRwuLGGae8VKpPc4jEwpGmvoGj8cfS2qoEMNPtRnGM3K
+t+q39zLoDk+6Kmr5oi8XVfZmibXRtNvrixMj6jAEm/3Vag9VdQ4SR+QFwpJOcIOB
+tX9mDnamXnBHWFqGUqOUU9/6y4p8B2o3RDE/WeiWtU66gQZasli6TJb0RpNoY/Xy
+XHGn+J0gd9EDXn0CAwEAAaMyMDAwDwYDVR0TAQH/BAUwAwEB/zAdBgNVHQ4EFgQU
+82QyfbI8XeUu4El8tOpiFZR4LqswDQYJKoZIhvcNAQELBQADggIBAI3hBTzed1Zt
+Dh5DvdidSJoGRBXJQ24Y3VjxPbelLNxnZiYCiSIQhL7KIjmDZOBQJwqlBxWOsao7
+PuRaohdAcDQ2jImeiIAmkRaTcUWZgB++IuS1ta01XMcAEp/taQEjHKjwAr22IILN
+Vk9z0WNVf5Pd9NWMu4lFqwECpKTJnToIqEGVVWcqAAupGT64LQ/Cf+/oEpDtkRaV
+azFj7ob1Rxjl5hmOxMwNHW8wRPcq8glg+26Tp9jqcaw32fhfnUPDHBdoYcU/VhMk
+gBeYXGHTPHp32Kj4l/QxWnxY0IvChyq+Qao1D19K5PbJQH5A5bQbwqgBtMihsdrG
+Sr9VJ7LtNmBc+8dNchqi2uXs3ryk8htDluZ60yWK89eRO1NatB2tiDLh5iwejJRi
+eOoyQ3Iq8m/IjtEJTs7ehWJHtiGj2U/tlpVW2fSszoz0TbKxXQPQ/dGNmDorqrM/
+0WEY6lkNEp7qbXB1U378PFUKFh1lIdlfNrgoEvYt0XeIMbXn+fUkB8munP0bCSiJ
+qX7gK+2FuZqfA038JfuwxDBr8SvkkvZOqyUgMPAPRpQCjmFrZgMrilHUokZIL5+C
+z4qaxEf3s3xORy+CuPMousfrOKpdf6jFjnyD8cr4Ez4bMAekPg4F4JJ0WHpOchSl
+DP5a57cb6mHYvOF8ygSobADyNeQ1jkjg
+-----END CERTIFICATE-----
+                            "</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -131,7 +206,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -143,7 +218,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -190,6 +265,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -225,6 +317,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,17 +485,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="46.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="3.9140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="46.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -403,18 +512,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>